<commit_message>
add assemble explanation and photos
</commit_message>
<xml_diff>
--- a/20130725_Wave_Clock_PIC32MX130_Mono_PartsList.xlsx
+++ b/20130725_Wave_Clock_PIC32MX130_Mono_PartsList.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="143">
   <si>
     <t>Parts List for</t>
   </si>
@@ -192,9 +192,6 @@
   </si>
   <si>
     <t>IC3</t>
-  </si>
-  <si>
-    <t>NJM8202R</t>
   </si>
   <si>
     <t>MSOP08</t>
@@ -496,6 +493,17 @@
       </rPr>
       <t xml:space="preserve">  10K(A)</t>
     </r>
+    <phoneticPr fontId="23"/>
+  </si>
+  <si>
+    <t>NJM8202R / LMV358QDGKR(12TI RHR)</t>
+    <phoneticPr fontId="23"/>
+  </si>
+  <si>
+    <t>秋月電子通商 / RSコンポーネンツ</t>
+    <rPh sb="0" eb="6">
+      <t>アキヅキ</t>
+    </rPh>
     <phoneticPr fontId="23"/>
   </si>
 </sst>
@@ -1696,14 +1704,14 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -2046,8 +2054,8 @@
   </sheetPr>
   <dimension ref="A1:D89"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="B80" sqref="B80"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2060,21 +2068,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="28.5" hidden="1" customHeight="1">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
     </row>
     <row r="2" spans="1:4" hidden="1"/>
     <row r="3" spans="1:4" ht="57" hidden="1" customHeight="1">
-      <c r="A3" s="56" t="s">
+      <c r="A3" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="57"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
+      <c r="B3" s="58"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
     </row>
     <row r="4" spans="1:4" hidden="1"/>
     <row r="5" spans="1:4" hidden="1">
@@ -2105,7 +2113,7 @@
         <v>5</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="14.25" thickBot="1">
@@ -2119,7 +2127,7 @@
         <v>19</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -2133,7 +2141,7 @@
         <v>1608</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -2147,7 +2155,7 @@
         <v>1608</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -2161,7 +2169,7 @@
         <v>1608</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -2175,7 +2183,7 @@
         <v>1608</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -2189,7 +2197,7 @@
         <v>1608</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -2203,7 +2211,7 @@
         <v>1608</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -2217,7 +2225,7 @@
         <v>1608</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="14.25" thickBot="1">
@@ -2231,7 +2239,7 @@
         <v>1608</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -2245,7 +2253,7 @@
         <v>1608</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -2259,7 +2267,7 @@
         <v>1608</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -2273,7 +2281,7 @@
         <v>1608</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="14.25" thickBot="1">
@@ -2287,7 +2295,7 @@
         <v>1608</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -2301,7 +2309,7 @@
         <v>3216</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -2315,7 +2323,7 @@
         <v>3216</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -2329,7 +2337,7 @@
         <v>3216</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -2343,7 +2351,7 @@
         <v>3216</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -2357,7 +2365,7 @@
         <v>3216</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="14.25" thickBot="1">
@@ -2371,7 +2379,7 @@
         <v>3216</v>
       </c>
       <c r="D28" s="18" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -2385,7 +2393,7 @@
         <v>1608</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="14.25" thickBot="1">
@@ -2399,7 +2407,7 @@
         <v>1608</v>
       </c>
       <c r="D30" s="18" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -2413,7 +2421,7 @@
         <v>1608</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="14.25" thickBot="1">
@@ -2427,7 +2435,7 @@
         <v>1608</v>
       </c>
       <c r="D32" s="23" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -2441,7 +2449,7 @@
         <v>8</v>
       </c>
       <c r="D33" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -2455,7 +2463,7 @@
         <v>8</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -2469,7 +2477,7 @@
         <v>8</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -2483,7 +2491,7 @@
         <v>8</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -2497,7 +2505,7 @@
         <v>46</v>
       </c>
       <c r="D37" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -2511,7 +2519,7 @@
         <v>48</v>
       </c>
       <c r="D38" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="14.25" thickBot="1">
@@ -2525,7 +2533,7 @@
         <v>41</v>
       </c>
       <c r="D39" s="18" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -2539,7 +2547,7 @@
         <v>53</v>
       </c>
       <c r="D40" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -2553,7 +2561,7 @@
         <v>56</v>
       </c>
       <c r="D41" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -2567,7 +2575,7 @@
         <v>56</v>
       </c>
       <c r="D42" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -2575,74 +2583,74 @@
         <v>58</v>
       </c>
       <c r="B43" s="32" t="s">
+        <v>141</v>
+      </c>
+      <c r="C43" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="C43" s="9" t="s">
-        <v>60</v>
-      </c>
       <c r="D43" s="15" t="s">
-        <v>121</v>
+        <v>142</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B44" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="B44" s="32" t="s">
+      <c r="C44" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C44" s="9" t="s">
-        <v>63</v>
-      </c>
       <c r="D44" s="15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B45" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="C45" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="B45" s="32" t="s">
-        <v>124</v>
-      </c>
-      <c r="C45" s="9" t="s">
-        <v>65</v>
-      </c>
       <c r="D45" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B46" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="B46" s="32" t="s">
+      <c r="C46" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C46" s="9" t="s">
-        <v>68</v>
-      </c>
       <c r="D46" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="14.25" thickBot="1">
       <c r="A47" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B47" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="B47" s="33" t="s">
+      <c r="C47" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="C47" s="17" t="s">
-        <v>71</v>
-      </c>
       <c r="D47" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B48" s="31">
         <v>10</v>
@@ -2651,12 +2659,12 @@
         <v>1608</v>
       </c>
       <c r="D48" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="14.25" thickBot="1">
       <c r="A49" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B49" s="34">
         <v>100</v>
@@ -2665,455 +2673,455 @@
         <v>1608</v>
       </c>
       <c r="D49" s="23" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B50" s="31" t="s">
         <v>72</v>
-      </c>
-      <c r="B50" s="31" t="s">
-        <v>73</v>
       </c>
       <c r="C50" s="12">
         <v>1608</v>
       </c>
       <c r="D50" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B51" s="32" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C51" s="9">
         <v>1608</v>
       </c>
       <c r="D51" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B52" s="32" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C52" s="9">
         <v>1608</v>
       </c>
       <c r="D52" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B53" s="32" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C53" s="9">
         <v>1608</v>
       </c>
       <c r="D53" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B54" s="32" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C54" s="9">
         <v>1608</v>
       </c>
       <c r="D54" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B55" s="32" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C55" s="9">
         <v>1608</v>
       </c>
       <c r="D55" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B56" s="32" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C56" s="9">
         <v>1608</v>
       </c>
       <c r="D56" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="14.25" thickBot="1">
       <c r="A57" s="16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B57" s="33" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C57" s="17">
         <v>1608</v>
       </c>
       <c r="D57" s="18" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B58" s="31" t="s">
         <v>74</v>
-      </c>
-      <c r="B58" s="31" t="s">
-        <v>75</v>
       </c>
       <c r="C58" s="12">
         <v>1608</v>
       </c>
       <c r="D58" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B59" s="32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C59" s="9">
         <v>1608</v>
       </c>
       <c r="D59" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B60" s="32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C60" s="9">
         <v>1608</v>
       </c>
       <c r="D60" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B61" s="32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C61" s="9">
         <v>1608</v>
       </c>
       <c r="D61" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B62" s="32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C62" s="9">
         <v>1608</v>
       </c>
       <c r="D62" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B63" s="32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C63" s="9">
         <v>1608</v>
       </c>
       <c r="D63" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B64" s="32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C64" s="9">
         <v>1608</v>
       </c>
       <c r="D64" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B65" s="32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C65" s="9">
         <v>1608</v>
       </c>
       <c r="D65" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B66" s="32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C66" s="9">
         <v>1608</v>
       </c>
       <c r="D66" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B67" s="32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C67" s="9">
         <v>1608</v>
       </c>
       <c r="D67" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="14.25" thickBot="1">
       <c r="A68" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B68" s="33" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C68" s="17">
         <v>1608</v>
       </c>
       <c r="D68" s="18" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="14.25" thickBot="1">
       <c r="A69" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="B69" s="35" t="s">
         <v>90</v>
-      </c>
-      <c r="B69" s="35" t="s">
-        <v>91</v>
       </c>
       <c r="C69" s="25">
         <v>1608</v>
       </c>
       <c r="D69" s="26" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B70" s="31" t="s">
         <v>84</v>
-      </c>
-      <c r="B70" s="31" t="s">
-        <v>85</v>
       </c>
       <c r="C70" s="12">
         <v>1608</v>
       </c>
       <c r="D70" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B71" s="32" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C71" s="9">
         <v>1608</v>
       </c>
       <c r="D71" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="14.25" thickBot="1">
       <c r="A72" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B72" s="33" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C72" s="17">
         <v>1608</v>
       </c>
       <c r="D72" s="18" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="14.25" thickBot="1">
       <c r="A73" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="B73" s="35" t="s">
+        <v>124</v>
+      </c>
+      <c r="C73" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="B73" s="35" t="s">
-        <v>125</v>
-      </c>
-      <c r="C73" s="25" t="s">
-        <v>102</v>
-      </c>
       <c r="D73" s="26" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="B74" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="B74" s="31" t="s">
+      <c r="C74" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="C74" s="12" t="s">
-        <v>105</v>
-      </c>
       <c r="D74" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B75" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="C75" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="C75" s="9" t="s">
-        <v>105</v>
-      </c>
       <c r="D75" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B76" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="C76" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="C76" s="9" t="s">
-        <v>105</v>
-      </c>
       <c r="D76" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="14.25" thickBot="1">
       <c r="A77" s="16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B77" s="33" t="s">
+        <v>103</v>
+      </c>
+      <c r="C77" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="C77" s="17" t="s">
-        <v>105</v>
-      </c>
       <c r="D77" s="18" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="B78" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="B78" s="31" t="s">
+      <c r="C78" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="C78" s="12" t="s">
-        <v>111</v>
-      </c>
       <c r="D78" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="14.25" thickBot="1">
       <c r="A79" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B79" s="33" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C79" s="17" t="s">
         <v>53</v>
       </c>
       <c r="D79" s="18" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="14.25" thickBot="1">
       <c r="A80" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="B80" s="56" t="s">
+        <v>140</v>
+      </c>
+      <c r="C80" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="B80" s="58" t="s">
-        <v>141</v>
-      </c>
-      <c r="C80" s="25" t="s">
-        <v>114</v>
-      </c>
       <c r="D80" s="26" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="14.25" thickBot="1">
       <c r="A81" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="B81" s="35" t="s">
         <v>115</v>
       </c>
-      <c r="B81" s="35" t="s">
-        <v>116</v>
-      </c>
       <c r="C81" s="25" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D81" s="26" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -3121,24 +3129,24 @@
     </row>
     <row r="83" spans="1:4" hidden="1">
       <c r="A83" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="84" spans="1:4" hidden="1">
       <c r="A84" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="85" spans="1:4" hidden="1">
       <c r="A85" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="86" spans="1:4" hidden="1"/>
     <row r="87" spans="1:4" hidden="1"/>
     <row r="88" spans="1:4">
       <c r="B88" s="36" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C88" s="36">
         <v>1</v>
@@ -3146,7 +3154,7 @@
     </row>
     <row r="89" spans="1:4">
       <c r="B89" s="36" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C89" s="36">
         <v>1</v>
@@ -3264,7 +3272,7 @@
       <c r="E3" s="41"/>
       <c r="F3" s="41"/>
       <c r="G3" s="41" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H3" s="41"/>
       <c r="I3" s="41"/>
@@ -3278,7 +3286,7 @@
       <c r="Q3" s="41"/>
       <c r="R3" s="41"/>
       <c r="S3" s="41" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="T3" s="41"/>
       <c r="U3" s="41"/>
@@ -3292,7 +3300,7 @@
       <c r="AC3" s="41"/>
       <c r="AD3" s="41"/>
       <c r="AE3" s="41" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AF3" s="41"/>
       <c r="AG3" s="41"/>
@@ -3764,7 +3772,7 @@
       <c r="E16" s="41"/>
       <c r="F16" s="41"/>
       <c r="G16" s="41" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H16" s="41"/>
       <c r="I16" s="41"/>
@@ -3778,7 +3786,7 @@
       <c r="Q16" s="41"/>
       <c r="R16" s="41"/>
       <c r="S16" s="41" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="T16" s="41"/>
       <c r="U16" s="41"/>
@@ -4261,7 +4269,7 @@
       <c r="D29" s="41"/>
       <c r="E29" s="41"/>
       <c r="F29" s="41" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G29" s="41"/>
       <c r="H29" s="41"/>
@@ -4276,7 +4284,7 @@
       <c r="Q29" s="41"/>
       <c r="R29" s="41"/>
       <c r="S29" s="41" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="T29" s="41"/>
       <c r="U29" s="41"/>
@@ -4290,7 +4298,7 @@
       <c r="AC29" s="41"/>
       <c r="AD29" s="41"/>
       <c r="AE29" s="41" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="AF29" s="41"/>
       <c r="AG29" s="41"/>
@@ -4761,7 +4769,7 @@
       <c r="D42" s="41"/>
       <c r="E42" s="41"/>
       <c r="F42" s="41" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G42" s="41"/>
       <c r="H42" s="41"/>
@@ -4776,7 +4784,7 @@
       <c r="Q42" s="41"/>
       <c r="R42" s="41"/>
       <c r="S42" s="41" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="T42" s="41"/>
       <c r="U42" s="41"/>
@@ -4790,7 +4798,7 @@
       <c r="AC42" s="41"/>
       <c r="AD42" s="41"/>
       <c r="AE42" s="41" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AF42" s="41"/>
       <c r="AG42" s="41"/>

</xml_diff>